<commit_message>
FRED data series are prepared
</commit_message>
<xml_diff>
--- a/PROJECT_FOMC/fred/FOMC_FRED_DATAMASTER.xlsx
+++ b/PROJECT_FOMC/fred/FOMC_FRED_DATAMASTER.xlsx
@@ -257,6 +257,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -277,24 +278,28 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF262626"/>
       <name val="Verdana-Bold"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF262626"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -339,7 +344,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -374,6 +379,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -453,13 +462,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J18"/>
+  <dimension ref="A2:J23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.67"/>
@@ -536,7 +545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="110.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="87.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -568,7 +577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="218.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="174.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -632,7 +641,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="94.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="190.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -790,11 +799,19 @@
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
     </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1" display="https://fred.stlouisfed.org/series/UNRATE"/>
-    <hyperlink ref="C8" r:id="rId2" display="Bureau of Economic Analysis"/>
-    <hyperlink ref="C9" r:id="rId3" display="Wilshire Associates"/>
+    <hyperlink ref="C8" r:id="rId2" display="Real gross domestic product is the inflation adjusted value of the goods and services produced by labor and property located in the United States.For more information see the Guide to the National Income and Product Accounts of the United States (NIPA). For more information, please visit the Bureau of Economic Analysis."/>
+    <hyperlink ref="C9" r:id="rId3" display="The observations for the Wilshire 5000 Total Market Index represent the daily index value at market close. The market typically closes at 4 PM ET, except for holidays when it sometimes closes early. + +The total market indexes are total market returns, which do include reinvested dividends. Copyright, 2016, Wilshire Associates Incorporated. Reprinted with permission. For more information about the various indexes, visit Wilshire Associates."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updated data to May 9, 2022. Removed GDPC1
</commit_message>
<xml_diff>
--- a/PROJECT_FOMC/fred/FOMC_FRED_DATAMASTER.xlsx
+++ b/PROJECT_FOMC/fred/FOMC_FRED_DATAMASTER.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t xml:space="preserve">Financial Data Series from FRED</t>
   </si>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">2006/12/29</t>
   </si>
   <si>
-    <t xml:space="preserve">2022/04/25</t>
+    <t xml:space="preserve">2022/05/10</t>
   </si>
   <si>
     <t xml:space="preserve">https://fred.stlouisfed.org/series/T10YIE</t>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">2006/12/01</t>
   </si>
   <si>
-    <t xml:space="preserve">2022/03/01</t>
+    <t xml:space="preserve">2022/04/01</t>
   </si>
   <si>
     <t xml:space="preserve">https://fred.stlouisfed.org/series/UNRATE</t>
@@ -139,33 +139,6 @@
     <t xml:space="preserve">CIVPART.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Real Gross Domestic Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDPC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Real gross domestic product is the inflation adjusted value of the goods and services produced by labor and property located in the United States.For more information see the Guide to the National Income and Product Accounts of the United States (NIPA). For more information, please visit the Bureau of Economic Analysis.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDPC1.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quarterly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billions of Chained 2012 Dollars, Seasonally Adjusted Annual Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2006/10/01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021/10/01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://fred.stlouisfed.org/series/GDPC1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wilshire 5000 Total Market Index</t>
   </si>
   <si>
@@ -183,7 +156,7 @@
     <t xml:space="preserve">Index</t>
   </si>
   <si>
-    <t xml:space="preserve">2022/04/26</t>
+    <t xml:space="preserve">2022/05/09</t>
   </si>
   <si>
     <t xml:space="preserve">https://fred.stlouisfed.org/series/WILL5000IND</t>
@@ -208,7 +181,7 @@
     <t xml:space="preserve">Index 2012=100</t>
   </si>
   <si>
-    <t xml:space="preserve">2022/02/01</t>
+    <t xml:space="preserve">2022/03/01</t>
   </si>
   <si>
     <t xml:space="preserve">https://fred.stlouisfed.org/series/PCEPILFE</t>
@@ -239,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">DGS10.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/04/25</t>
   </si>
   <si>
     <t xml:space="preserve">https://fred.stlouisfed.org/series/DGS10</t>
@@ -344,7 +320,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,10 +347,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -462,13 +434,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J23"/>
+  <dimension ref="A2:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.67"/>
@@ -609,7 +581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="70.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="190.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -623,100 +595,100 @@
         <v>37</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="J8" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="204.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="190.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>27</v>
       </c>
       <c r="I9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="39.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="204.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E10" s="0" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="39.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>15</v>
@@ -731,43 +703,16 @@
         <v>27</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>66</v>
-      </c>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
@@ -794,22 +739,16 @@
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="D18" s="2"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9"/>
+      <c r="A22" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1" display="https://fred.stlouisfed.org/series/UNRATE"/>
-    <hyperlink ref="C8" r:id="rId2" display="Real gross domestic product is the inflation adjusted value of the goods and services produced by labor and property located in the United States.For more information see the Guide to the National Income and Product Accounts of the United States (NIPA). For more information, please visit the Bureau of Economic Analysis."/>
-    <hyperlink ref="C9" r:id="rId3" display="The observations for the Wilshire 5000 Total Market Index represent the daily index value at market close. The market typically closes at 4 PM ET, except for holidays when it sometimes closes early. +    <hyperlink ref="C8" r:id="rId2" display="The observations for the Wilshire 5000 Total Market Index represent the daily index value at market close. The market typically closes at 4 PM ET, except for holidays when it sometimes closes early.    The total market indexes are total market returns, which do include reinvested dividends. Copyright, 2016, Wilshire Associates Incorporated. Reprinted with permission. For more information about the various indexes, visit Wilshire Associates."/>
   </hyperlinks>

</xml_diff>